<commit_message>
third commit GitHub modified Excel file test
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Redmond\PycharmProjects\test-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D50348-7AAF-4233-A1EB-56E0307CA326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89872E35-48BA-4AE8-8762-378AF3BC65CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0793179B-EB1B-4A3E-A28D-968EB64E05B4}"/>
   </bookViews>
@@ -34,9 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
-    <t>test</t>
+    <t>second test</t>
   </si>
 </sst>
 </file>
@@ -388,16 +388,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCEF7D3-645C-4873-A242-B2F4E5AFB467}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>